<commit_message>
dang chinh lai doan luu vao excel
</commit_message>
<xml_diff>
--- a/Data/test.xlsx
+++ b/Data/test.xlsx
@@ -10,7 +10,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="11028"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9612"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>tagName</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>StartTime</t>
-  </si>
-  <si>
-    <t>Step</t>
   </si>
   <si>
     <t>ATTT</t>
@@ -192,9 +189,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -476,13 +472,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,242 +500,203 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1">
-        <v>44055.457627314812</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44056</v>
+        <v>44066</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1">
+        <v>44067</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
-        <v>44053.452175925922</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1">
+        <v>44068</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1">
-        <v>44053.452175925922</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1">
+        <v>44069</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1">
-        <v>44053.452175925922</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="1">
+        <v>44070</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1">
-        <v>44053.452175925922</v>
-      </c>
-      <c r="D6" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="1">
+        <v>44071</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1">
-        <v>44053.43513888889</v>
-      </c>
-      <c r="D7" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1">
+        <v>44072</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1">
-        <v>44053.43513888889</v>
-      </c>
-      <c r="D8" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="1">
+        <v>44073</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="1">
-        <v>44053.43513888889</v>
-      </c>
-      <c r="D9" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="1">
+        <v>44074</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1">
-        <v>44053.43513888889</v>
-      </c>
-      <c r="D10" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1">
+        <v>44075</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="1">
-        <v>44053.435150462959</v>
-      </c>
-      <c r="D11" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="1">
+        <v>44076</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1">
-        <v>44053.435150462959</v>
-      </c>
-      <c r="D12" s="2">
-        <v>44044</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="1">
+        <v>44066</v>
+      </c>
+      <c r="F13" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="2">
-        <v>44044</v>
-      </c>
-      <c r="D13" s="2">
-        <v>44044</v>
       </c>
       <c r="G13" t="s">
         <v>42</v>
-      </c>
-      <c r="H13" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>